<commit_message>
sửa feedback và check lỗi
</commit_message>
<xml_diff>
--- a/temp/Getsu/Resources/ErrorGetsu.xlsx
+++ b/temp/Getsu/Resources/ErrorGetsu.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AD$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Tên file ảnh (Đường dẫn\tên batch\tên file ảnh)</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>16.通貨によるものの額5月</t>
+  </si>
+  <si>
+    <t>Flag</t>
   </si>
 </sst>
 </file>
@@ -484,13 +487,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +503,7 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,12 +591,15 @@
       <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD1"/>
+  <autoFilter ref="A1:AE1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>